<commit_message>
all charts are a go
</commit_message>
<xml_diff>
--- a/Scoring Algorithm Study and Charts.xlsx
+++ b/Scoring Algorithm Study and Charts.xlsx
@@ -2093,6 +2093,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Score for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> POI Count within Radius</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2325,157 +2355,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.0758581800212434</c:v>
+                  <c:v>0.758581800212434</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.119202922022118</c:v>
+                  <c:v>1.192029220221176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.182425523806356</c:v>
+                  <c:v>1.824255238063564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.268941421369995</c:v>
+                  <c:v>2.689414213699951</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.377540668798145</c:v>
+                  <c:v>3.775406687981454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.622459331201854</c:v>
+                  <c:v>6.224593312018546</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.731058578630005</c:v>
+                  <c:v>7.310585786300049</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.817574476193644</c:v>
+                  <c:v>8.175744761936435</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.880797077977882</c:v>
+                  <c:v>8.807970779778824</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.924141819978756</c:v>
+                  <c:v>9.241418199787564</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.952574126822433</c:v>
+                  <c:v>9.52574126822433</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.970687769248644</c:v>
+                  <c:v>9.706877692486437</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.982013790037908</c:v>
+                  <c:v>9.820137900379084</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.989013057369407</c:v>
+                  <c:v>9.890130573694067</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.993307149075715</c:v>
+                  <c:v>9.933071490757152</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.995929862284104</c:v>
+                  <c:v>9.95929862284104</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.997527376843365</c:v>
+                  <c:v>9.975273768433652</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.998498817743263</c:v>
+                  <c:v>9.98498817743263</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.999088948805599</c:v>
+                  <c:v>9.990889488055993</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.999447221363076</c:v>
+                  <c:v>9.994472213630764</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.999664649869533</c:v>
+                  <c:v>9.996646498695335</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.999796573021945</c:v>
+                  <c:v>9.997965730219448</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.999876605424014</c:v>
+                  <c:v>9.998766054240137</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.999925153772489</c:v>
+                  <c:v>9.999251537724893</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.999954602131298</c:v>
+                  <c:v>9.999546021312974</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.999972464308885</c:v>
+                  <c:v>9.999724643088853</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.999983298578152</c:v>
+                  <c:v>9.999832985781518</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.999989870009019</c:v>
+                  <c:v>9.999898700090192</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.999993855825398</c:v>
+                  <c:v>9.999938558253978</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.999996273360716</c:v>
+                  <c:v>9.999962733607157</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.999997739675702</c:v>
+                  <c:v>9.999977396757021</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.999998629042793</c:v>
+                  <c:v>9.99998629042793</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.999999168471972</c:v>
+                  <c:v>9.999991684719724</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.999999495652592</c:v>
+                  <c:v>9.999994956525917</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.999999694097773</c:v>
+                  <c:v>9.99999694097773</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.999999814460898</c:v>
+                  <c:v>9.999998144608982</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.999999887464838</c:v>
+                  <c:v>9.99999887464838</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.999999931743971</c:v>
+                  <c:v>9.999999317439708</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.999999958600624</c:v>
+                  <c:v>9.999999586006245</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.999999974890009</c:v>
+                  <c:v>9.99999974890009</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.99999998477002</c:v>
+                  <c:v>9.999999847700204</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99999999076255</c:v>
+                  <c:v>9.999999907625504</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.999999994397204</c:v>
+                  <c:v>9.999999943972035</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.999999996601732</c:v>
+                  <c:v>9.999999966017321</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.999999997938846</c:v>
+                  <c:v>9.999999979388464</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.999999998749847</c:v>
+                  <c:v>9.999999987498471</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.999999999241744</c:v>
+                  <c:v>9.99999999241744</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.999999999540094</c:v>
+                  <c:v>9.999999995400944</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.999999999721053</c:v>
+                  <c:v>9.999999997210531</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.99999999983081</c:v>
+                  <c:v>9.9999999983081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2497,6 +2527,7 @@
         <c:axId val="108790032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2514,6 +2545,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Point of Interest Count within Radius</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2554,11 +2642,14 @@
         <c:crossAx val="189847264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="189847264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10.1"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2576,6 +2667,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2616,6 +2763,7 @@
         <c:crossAx val="108790032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5736,8 +5884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5938,12 +6086,12 @@
         <v>0.5</v>
       </c>
       <c r="R9">
-        <f>1-1/(1+EXP(-Q9*(P9-N9)))</f>
-        <v>7.5858180021243449E-2</v>
+        <f>10-10/(1+EXP(-Q9*(P9-N9)))</f>
+        <v>0.75858180021243449</v>
       </c>
       <c r="T9">
         <f>SUM(R9*O9,L9*I9,F9*C9)/SUM(O9,I9,C9)</f>
-        <v>6.6131371649512118</v>
+        <v>6.8407117050149431</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -5997,12 +6145,12 @@
         <v>0.5</v>
       </c>
       <c r="R10">
-        <f t="shared" ref="R10:R73" si="4">1-1/(1+EXP(-Q10*(P10-N10)))</f>
-        <v>0.11920292202211769</v>
+        <f t="shared" ref="R10:R73" si="4">10-10/(1+EXP(-Q10*(P10-N10)))</f>
+        <v>1.1920292202211762</v>
       </c>
       <c r="T10">
         <f t="shared" ref="T10:T73" si="5">SUM(R10*O10,L10*I10,F10*C10)/SUM(O10,I10,C10)</f>
-        <v>6.6168541704429105</v>
+        <v>6.9744629365092647</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -6057,11 +6205,11 @@
       </c>
       <c r="R11">
         <f t="shared" si="4"/>
-        <v>0.18242552380635635</v>
+        <v>1.8242552380635644</v>
       </c>
       <c r="T11">
         <f t="shared" si="5"/>
-        <v>6.6032465702000636</v>
+        <v>7.1505231416191322</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -6116,11 +6264,11 @@
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
-        <v>0.2689414213699951</v>
+        <v>2.6894142136999513</v>
       </c>
       <c r="T12">
         <f t="shared" si="5"/>
-        <v>6.593468379962121</v>
+        <v>7.4002926440721062</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -6175,11 +6323,11 @@
       </c>
       <c r="R13">
         <f t="shared" si="4"/>
-        <v>0.37754066879814541</v>
+        <v>3.7754066879814543</v>
       </c>
       <c r="T13">
         <f t="shared" si="5"/>
-        <v>6.5863450142708091</v>
+        <v>7.7189670206652456</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -6234,11 +6382,11 @@
       </c>
       <c r="R14">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="T14">
         <f t="shared" si="5"/>
-        <v>6.5781909419136619</v>
+        <v>8.0781909419136628</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -6293,11 +6441,11 @@
       </c>
       <c r="R15">
         <f t="shared" si="4"/>
-        <v>0.62245933120185459</v>
+        <v>6.2245933120185457</v>
       </c>
       <c r="T15">
         <f t="shared" si="5"/>
-        <v>6.5632404020811634</v>
+        <v>8.4306183956867269</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -6352,11 +6500,11 @@
       </c>
       <c r="R16">
         <f t="shared" si="4"/>
-        <v>0.7310585786300049</v>
+        <v>7.3105857863000487</v>
       </c>
       <c r="T16">
         <f t="shared" si="5"/>
-        <v>6.535501766906485</v>
+        <v>8.7286775027964989</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -6411,11 +6559,11 @@
       </c>
       <c r="R17">
         <f t="shared" si="4"/>
-        <v>0.81757447619364365</v>
+        <v>8.1757447619364356</v>
       </c>
       <c r="T17">
         <f t="shared" si="5"/>
-        <v>6.49062184261357</v>
+        <v>8.9433452711945005</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -6470,11 +6618,11 @@
       </c>
       <c r="R18">
         <f t="shared" si="4"/>
-        <v>0.88079707797788243</v>
+        <v>8.8079707797788238</v>
       </c>
       <c r="T18">
         <f t="shared" si="5"/>
-        <v>6.4263498037114184</v>
+        <v>9.068741037645065</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -6529,11 +6677,11 @@
       </c>
       <c r="R19">
         <f t="shared" si="4"/>
-        <v>0.92414181997875644</v>
+        <v>9.2414181997875637</v>
       </c>
       <c r="T19">
         <f t="shared" si="5"/>
-        <v>6.3417797556997426</v>
+        <v>9.1142052156360123</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -6588,11 +6736,11 @@
       </c>
       <c r="R20">
         <f t="shared" si="4"/>
-        <v>0.95257412682243325</v>
+        <v>9.5257412682243316</v>
       </c>
       <c r="T20">
         <f t="shared" si="5"/>
-        <v>6.2364147031317758</v>
+        <v>9.094137083599076</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -6647,11 +6795,11 @@
       </c>
       <c r="R21">
         <f t="shared" si="4"/>
-        <v>0.97068776924864364</v>
+        <v>9.7068776924864366</v>
       </c>
       <c r="T21">
         <f t="shared" si="5"/>
-        <v>6.1096836339936607</v>
+        <v>9.0217469417395915</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -6706,11 +6854,11 @@
       </c>
       <c r="R22">
         <f t="shared" si="4"/>
-        <v>0.98201379003790845</v>
+        <v>9.8201379003790841</v>
       </c>
       <c r="T22">
         <f t="shared" si="5"/>
-        <v>5.9609503197027465</v>
+        <v>8.906991689816472</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -6765,11 +6913,11 @@
       </c>
       <c r="R23">
         <f t="shared" si="4"/>
-        <v>0.98901305736940681</v>
+        <v>9.8901305736940675</v>
       </c>
       <c r="T23">
         <f t="shared" si="5"/>
-        <v>5.7898297481017709</v>
+        <v>8.7568689202099907</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -6824,11 +6972,11 @@
       </c>
       <c r="R24">
         <f t="shared" si="4"/>
-        <v>0.99330714907571516</v>
+        <v>9.9330714907571522</v>
       </c>
       <c r="T24">
         <f t="shared" si="5"/>
-        <v>5.5966349640724191</v>
+        <v>8.5765564112995651</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -6883,11 +7031,11 @@
       </c>
       <c r="R25">
         <f t="shared" si="4"/>
-        <v>0.99592986228410385</v>
+        <v>9.9592986228410396</v>
       </c>
       <c r="T25">
         <f t="shared" si="5"/>
-        <v>5.382816489139949</v>
+        <v>8.3706060759922618</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -6942,11 +7090,11 @@
       </c>
       <c r="R26">
         <f t="shared" si="4"/>
-        <v>0.99752737684336523</v>
+        <v>9.9752737684336523</v>
       </c>
       <c r="T26">
         <f t="shared" si="5"/>
-        <v>5.1512712676289736</v>
+        <v>8.1438533981590684</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -7001,11 +7149,11 @@
       </c>
       <c r="R27">
         <f t="shared" si="4"/>
-        <v>0.99849881774326299</v>
+        <v>9.9849881774326299</v>
       </c>
       <c r="T27">
         <f t="shared" si="5"/>
-        <v>4.9064093479981361</v>
+        <v>7.901905801227926</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -7060,11 +7208,11 @@
       </c>
       <c r="R28">
         <f t="shared" si="4"/>
-        <v>0.9990889488055994</v>
+        <v>9.9908894880559931</v>
       </c>
       <c r="T28">
         <f t="shared" si="5"/>
-        <v>4.6539077927352146</v>
+        <v>7.6511746391520115</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -7119,11 +7267,11 @@
       </c>
       <c r="R29">
         <f t="shared" si="4"/>
-        <v>0.9994472213630764</v>
+        <v>9.9944722136307647</v>
       </c>
       <c r="T29">
         <f t="shared" si="5"/>
-        <v>4.4001642105778425</v>
+        <v>7.3985058746670731</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -7178,11 +7326,11 @@
       </c>
       <c r="R30">
         <f t="shared" si="4"/>
-        <v>0.99966464986953352</v>
+        <v>9.9966464986953358</v>
       </c>
       <c r="T30">
         <f t="shared" si="5"/>
-        <v>4.1515628713198103</v>
+        <v>7.1505568209284105</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -7237,11 +7385,11 @@
       </c>
       <c r="R31">
         <f t="shared" si="4"/>
-        <v>0.9997965730219448</v>
+        <v>9.9979657302194482</v>
       </c>
       <c r="T31">
         <f t="shared" si="5"/>
-        <v>3.9137360574756435</v>
+        <v>6.9131257765414773</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -7296,11 +7444,11 @@
       </c>
       <c r="R32">
         <f t="shared" si="4"/>
-        <v>0.9998766054240138</v>
+        <v>9.9987660542401375</v>
       </c>
       <c r="T32">
         <f t="shared" si="5"/>
-        <v>3.6910023899264939</v>
+        <v>6.6906322061985355</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -7355,11 +7503,11 @@
       </c>
       <c r="R33">
         <f t="shared" si="4"/>
-        <v>0.99992515377248936</v>
+        <v>9.9992515377248932</v>
       </c>
       <c r="T33">
         <f t="shared" si="5"/>
-        <v>3.4860923905848282</v>
+        <v>6.4858678519022961</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -7414,11 +7562,11 @@
       </c>
       <c r="R34">
         <f t="shared" si="4"/>
-        <v>0.99995460213129761</v>
+        <v>9.999546021312975</v>
       </c>
       <c r="T34">
         <f t="shared" si="5"/>
-        <v>3.3001696396130664</v>
+        <v>6.3000334460069594</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -7473,11 +7621,11 @@
       </c>
       <c r="R35">
         <f t="shared" si="4"/>
-        <v>0.99997246430888542</v>
+        <v>9.9997246430888538</v>
       </c>
       <c r="T35">
         <f t="shared" si="5"/>
-        <v>3.1330735473471223</v>
+        <v>6.1329909402737783</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -7532,11 +7680,11 @@
       </c>
       <c r="R36">
         <f t="shared" si="4"/>
-        <v>0.99998329857815194</v>
+        <v>9.9998329857815182</v>
       </c>
       <c r="T36">
         <f t="shared" si="5"/>
-        <v>2.9836749724280871</v>
+        <v>5.9836248681625435</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -7591,11 +7739,11 @@
       </c>
       <c r="R37">
         <f t="shared" si="4"/>
-        <v>0.99998987000901918</v>
+        <v>9.999898700090192</v>
       </c>
       <c r="T37">
         <f t="shared" si="5"/>
-        <v>2.8502457934857208</v>
+        <v>5.8502154035127782</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -7650,11 +7798,11 @@
       </c>
       <c r="R38">
         <f t="shared" si="4"/>
-        <v>0.99999385582539779</v>
+        <v>9.9999385582539784</v>
       </c>
       <c r="T38">
         <f t="shared" si="5"/>
-        <v>2.7307772814428048</v>
+        <v>5.730758848918998</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -7709,11 +7857,11 @@
       </c>
       <c r="R39">
         <f t="shared" si="4"/>
-        <v>0.99999627336071584</v>
+        <v>9.9999627336071573</v>
       </c>
       <c r="T39">
         <f t="shared" si="5"/>
-        <v>2.6232185489644508</v>
+        <v>5.6232073690465993</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -7768,11 +7916,11 @@
       </c>
       <c r="R40">
         <f t="shared" si="4"/>
-        <v>0.99999773967570205</v>
+        <v>9.9999773967570214</v>
       </c>
       <c r="T40">
         <f t="shared" si="5"/>
-        <v>2.5256333553451555</v>
+        <v>5.5256265743722617</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -7827,11 +7975,11 @@
       </c>
       <c r="R41">
         <f t="shared" si="4"/>
-        <v>0.99999862904279313</v>
+        <v>9.9999862904279322</v>
       </c>
       <c r="T41">
         <f t="shared" si="5"/>
-        <v>2.4362882940824302</v>
+        <v>5.4362841812108096</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -7886,11 +8034,11 @@
       </c>
       <c r="R42">
         <f t="shared" si="4"/>
-        <v>0.99999916847197234</v>
+        <v>9.9999916847197241</v>
       </c>
       <c r="T42">
         <f t="shared" si="5"/>
-        <v>2.3536903647076426</v>
+        <v>5.3536878701235606</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -7945,11 +8093,11 @@
       </c>
       <c r="R43">
         <f t="shared" si="4"/>
-        <v>0.99999949565259183</v>
+        <v>9.9999949565259172</v>
       </c>
       <c r="T43">
         <f t="shared" si="5"/>
-        <v>2.276591064917616</v>
+        <v>5.2765895518753911</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -8004,11 +8152,11 @@
       </c>
       <c r="R44">
         <f t="shared" si="4"/>
-        <v>0.99999969409777312</v>
+        <v>9.9999969409777307</v>
       </c>
       <c r="T44">
         <f t="shared" si="5"/>
-        <v>2.203970725193765</v>
+        <v>5.2039698074870842</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -8063,11 +8211,11 @@
       </c>
       <c r="R45">
         <f t="shared" si="4"/>
-        <v>0.99999981446089814</v>
+        <v>9.9999981446089823</v>
       </c>
       <c r="T45">
         <f t="shared" si="5"/>
-        <v>2.1350129017100499</v>
+        <v>5.1350123450927443</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -8122,11 +8270,11 @@
       </c>
       <c r="R46">
         <f t="shared" si="4"/>
-        <v>0.99999988746483792</v>
+        <v>9.9999988746483801</v>
       </c>
       <c r="T46">
         <f t="shared" si="5"/>
-        <v>2.0690752397288912</v>
+        <v>5.0690749021234049</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -8181,11 +8329,11 @@
       </c>
       <c r="R47">
         <f t="shared" si="4"/>
-        <v>0.99999993174397095</v>
+        <v>9.999999317439709</v>
       </c>
       <c r="T47">
         <f t="shared" si="5"/>
-        <v>2.0056606380295099</v>
+        <v>5.0056604332614221</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -8240,11 +8388,11 @@
       </c>
       <c r="R48">
         <f t="shared" si="4"/>
-        <v>0.99999995860062452</v>
+        <v>9.9999995860062452</v>
       </c>
       <c r="T48">
         <f t="shared" si="5"/>
-        <v>1.944390759850964</v>
+        <v>4.9443906356528373</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
@@ -8299,11 +8447,11 @@
       </c>
       <c r="R49">
         <f t="shared" si="4"/>
-        <v>0.99999997489000902</v>
+        <v>9.9999997489000911</v>
       </c>
       <c r="T49">
         <f t="shared" si="5"/>
-        <v>1.884982790122848</v>
+        <v>4.8849827147928755</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
@@ -8358,11 +8506,11 @@
       </c>
       <c r="R50">
         <f t="shared" si="4"/>
-        <v>0.9999999847700205</v>
+        <v>9.9999998477002041</v>
       </c>
       <c r="T50">
         <f t="shared" si="5"/>
-        <v>1.8272296544813489</v>
+        <v>4.8272296087914102</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
@@ -8417,11 +8565,11 @@
       </c>
       <c r="R51">
         <f t="shared" si="4"/>
-        <v>0.99999999076255042</v>
+        <v>9.9999999076255044</v>
       </c>
       <c r="T51">
         <f t="shared" si="5"/>
-        <v>1.7709835405906045</v>
+        <v>4.7709835128782556</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
@@ -8476,11 +8624,11 @@
       </c>
       <c r="R52">
         <f t="shared" si="4"/>
-        <v>0.99999999439720355</v>
+        <v>9.9999999439720355</v>
       </c>
       <c r="T52">
         <f t="shared" si="5"/>
-        <v>1.7161423824397373</v>
+        <v>4.7161423656313479</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
@@ -8535,11 +8683,11 @@
       </c>
       <c r="R53">
         <f t="shared" si="4"/>
-        <v>0.99999999660173222</v>
+        <v>9.999999966017322</v>
       </c>
       <c r="T53">
         <f t="shared" si="5"/>
-        <v>1.6626389045020324</v>
+        <v>4.6626388943072286</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -8594,11 +8742,11 @@
       </c>
       <c r="R54">
         <f t="shared" si="4"/>
-        <v>0.99999999793884642</v>
+        <v>9.9999999793884644</v>
       </c>
       <c r="T54">
         <f t="shared" si="5"/>
-        <v>1.6104318232835666</v>
+        <v>4.610431817100106</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
@@ -8653,11 +8801,11 @@
       </c>
       <c r="R55">
         <f t="shared" si="4"/>
-        <v>0.99999999874984713</v>
+        <v>9.9999999874984713</v>
       </c>
       <c r="T55">
         <f t="shared" si="5"/>
-        <v>1.5594988367471618</v>
+        <v>4.5594988329967032</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
@@ -8712,11 +8860,11 @@
       </c>
       <c r="R56">
         <f t="shared" si="4"/>
-        <v>0.99999999924174399</v>
+        <v>9.9999999924174396</v>
       </c>
       <c r="T56">
         <f t="shared" si="5"/>
-        <v>1.5098310783591025</v>
+        <v>4.5098310760843345</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
@@ -8771,11 +8919,11 @@
       </c>
       <c r="R57">
         <f t="shared" si="4"/>
-        <v>0.99999999954009444</v>
+        <v>9.9999999954009446</v>
       </c>
       <c r="T57">
         <f t="shared" si="5"/>
-        <v>1.4614287614342221</v>
+        <v>4.4614287600545053</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -8830,11 +8978,11 @@
       </c>
       <c r="R58">
         <f t="shared" si="4"/>
-        <v>0.99999999972105325</v>
+        <v>9.9999999972105318</v>
       </c>
       <c r="T58">
         <f t="shared" si="5"/>
-        <v>1.4142977855634147</v>
+        <v>4.4142977847265739</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
@@ -8889,11 +9037,11 @@
       </c>
       <c r="R59">
         <f t="shared" si="4"/>
-        <v>0.99999999983081023</v>
+        <v>9.9999999983081018</v>
       </c>
       <c r="T59">
         <f t="shared" si="5"/>
-        <v>1.3684471177502966</v>
+        <v>4.3684471172427273</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
@@ -8948,11 +9096,11 @@
       </c>
       <c r="R60">
         <f t="shared" si="4"/>
-        <v>0.9999999998973812</v>
+        <v>9.9999999989738129</v>
       </c>
       <c r="T60">
         <f t="shared" si="5"/>
-        <v>1.3238867957256784</v>
+        <v>4.3238867954178222</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
@@ -9007,11 +9155,11 @@
       </c>
       <c r="R61">
         <f t="shared" si="4"/>
-        <v>0.99999999993775857</v>
+        <v>9.9999999993775859</v>
       </c>
       <c r="T61">
         <f t="shared" si="5"/>
-        <v>1.2806264299156329</v>
+        <v>4.2806264297289083</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
@@ -9066,11 +9214,11 @@
       </c>
       <c r="R62">
         <f t="shared" si="4"/>
-        <v>0.99999999996224864</v>
+        <v>9.9999999996224869</v>
       </c>
       <c r="T62">
         <f t="shared" si="5"/>
-        <v>1.2386741043004352</v>
+        <v>4.2386741041871812</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -9125,11 +9273,11 @@
       </c>
       <c r="R63">
         <f t="shared" si="4"/>
-        <v>0.99999999997710265</v>
+        <v>9.9999999997710258</v>
       </c>
       <c r="T63">
         <f t="shared" si="5"/>
-        <v>1.1980355956597102</v>
+        <v>4.1980355955910182</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
@@ -9184,11 +9332,11 @@
       </c>
       <c r="R64">
         <f t="shared" si="4"/>
-        <v>0.99999999998611211</v>
+        <v>9.9999999998611209</v>
       </c>
       <c r="T64">
         <f t="shared" si="5"/>
-        <v>1.1587138462040258</v>
+        <v>4.1587138461623621</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
@@ -9243,11 +9391,11 @@
       </c>
       <c r="R65">
         <f t="shared" si="4"/>
-        <v>0.99999999999157652</v>
+        <v>9.9999999999157652</v>
       </c>
       <c r="T65">
         <f t="shared" si="5"/>
-        <v>1.1207086370324464</v>
+        <v>4.1207086370071755</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
@@ -9302,11 +9450,11 @@
       </c>
       <c r="R66">
         <f t="shared" si="4"/>
-        <v>0.99999999999489086</v>
+        <v>9.9999999999489084</v>
       </c>
       <c r="T66">
         <f t="shared" si="5"/>
-        <v>1.0840164198253086</v>
+        <v>4.0840164198099815</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
@@ -9361,11 +9509,11 @@
       </c>
       <c r="R67">
         <f t="shared" si="4"/>
-        <v>0.99999999999690115</v>
+        <v>9.9999999999690115</v>
       </c>
       <c r="T67">
         <f t="shared" si="5"/>
-        <v>1.0486302721806495</v>
+        <v>4.0486302721713523</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
@@ -9420,11 +9568,11 @@
       </c>
       <c r="R68">
         <f t="shared" si="4"/>
-        <v>0.9999999999981205</v>
+        <v>9.9999999999812044</v>
       </c>
       <c r="T68">
         <f t="shared" si="5"/>
-        <v>1.0145399484387785</v>
+        <v>4.0145399484331401</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
@@ -9479,11 +9627,11 @@
       </c>
       <c r="R69">
         <f t="shared" si="4"/>
-        <v>0.99999999999886002</v>
+        <v>9.9999999999885993</v>
       </c>
       <c r="T69">
         <f t="shared" si="5"/>
-        <v>0.9817320030397112</v>
+        <v>3.9817320030362908</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
@@ -9538,11 +9686,11 @@
       </c>
       <c r="R70">
         <f t="shared" si="4"/>
-        <v>0.99999999999930855</v>
+        <v>9.9999999999930864</v>
       </c>
       <c r="T70">
         <f t="shared" si="5"/>
-        <v>0.95018996768177921</v>
+        <v>3.9501899676797052</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -9597,11 +9745,11 @@
       </c>
       <c r="R71">
         <f t="shared" si="4"/>
-        <v>0.99999999999958067</v>
+        <v>9.999999999995806</v>
       </c>
       <c r="T71">
         <f t="shared" si="5"/>
-        <v>0.91989456700028682</v>
+        <v>3.9198945669990288</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
@@ -9656,11 +9804,11 @@
       </c>
       <c r="R72">
         <f t="shared" si="4"/>
-        <v>0.99999999999974565</v>
+        <v>9.9999999999974563</v>
       </c>
       <c r="T72">
         <f t="shared" si="5"/>
-        <v>0.89082396032122546</v>
+        <v>3.8908239603204624</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
@@ -9715,11 +9863,11 @@
       </c>
       <c r="R73">
         <f t="shared" si="4"/>
-        <v>0.99999999999984568</v>
+        <v>9.9999999999984563</v>
       </c>
       <c r="T73">
         <f t="shared" si="5"/>
-        <v>0.86295399938999118</v>
+        <v>3.8629539993895281</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
@@ -9773,12 +9921,12 @@
         <v>0.5</v>
       </c>
       <c r="R74">
-        <f t="shared" ref="R74:R137" si="10">1-1/(1+EXP(-Q74*(P74-N74)))</f>
-        <v>0.99999999999990641</v>
+        <f t="shared" ref="R74:R137" si="10">10-10/(1+EXP(-Q74*(P74-N74)))</f>
+        <v>9.9999999999990639</v>
       </c>
       <c r="T74">
         <f t="shared" ref="T74:T87" si="11">SUM(R74*O74,L74*I74,F74*C74)/SUM(O74,I74,C74)</f>
-        <v>0.83625849392414331</v>
+        <v>3.8362584939238622</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
@@ -9833,11 +9981,11 @@
       </c>
       <c r="R75">
         <f t="shared" si="10"/>
-        <v>0.99999999999994327</v>
+        <v>9.9999999999994316</v>
       </c>
       <c r="T75">
         <f t="shared" si="11"/>
-        <v>0.81070947846650554</v>
+        <v>3.8107094784663356</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
@@ -9892,11 +10040,11 @@
       </c>
       <c r="R76">
         <f t="shared" si="10"/>
-        <v>0.99999999999996558</v>
+        <v>9.9999999999996554</v>
       </c>
       <c r="T76">
         <f t="shared" si="11"/>
-        <v>0.78627747537781334</v>
+        <v>3.7862774753777102</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
@@ -9951,11 +10099,11 @@
       </c>
       <c r="R77">
         <f t="shared" si="10"/>
-        <v>0.99999999999997913</v>
+        <v>9.9999999999997904</v>
       </c>
       <c r="T77">
         <f t="shared" si="11"/>
-        <v>0.7629317499516951</v>
+        <v>3.7629317499516319</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
@@ -10010,11 +10158,11 @@
       </c>
       <c r="R78">
         <f t="shared" si="10"/>
-        <v>0.99999999999998734</v>
+        <v>9.9999999999998739</v>
       </c>
       <c r="T78">
         <f t="shared" si="11"/>
-        <v>0.74064055459456457</v>
+        <v>3.7406405545945272</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
@@ -10069,11 +10217,11 @@
       </c>
       <c r="R79">
         <f t="shared" si="10"/>
-        <v>0.99999999999999234</v>
+        <v>9.9999999999999236</v>
       </c>
       <c r="T79">
         <f t="shared" si="11"/>
-        <v>0.71937135981741329</v>
+        <v>3.7193713598173903</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
@@ -10128,11 +10276,11 @@
       </c>
       <c r="R80">
         <f t="shared" si="10"/>
-        <v>0.99999999999999534</v>
+        <v>9.9999999999999538</v>
       </c>
       <c r="T80">
         <f t="shared" si="11"/>
-        <v>0.69909107045852614</v>
+        <v>3.6990910704585125</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
@@ -10187,11 +10335,11 @@
       </c>
       <c r="R81">
         <f t="shared" si="10"/>
-        <v>0.99999999999999722</v>
+        <v>9.9999999999999716</v>
       </c>
       <c r="T81">
         <f t="shared" si="11"/>
-        <v>0.67976622611476289</v>
+        <v>3.6797662261147543</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
@@ -10246,11 +10394,11 @@
       </c>
       <c r="R82">
         <f t="shared" si="10"/>
-        <v>0.99999999999999833</v>
+        <v>9.9999999999999822</v>
       </c>
       <c r="T82">
         <f t="shared" si="11"/>
-        <v>0.66136318522008031</v>
+        <v>3.661363185220075</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
@@ -10305,11 +10453,11 @@
       </c>
       <c r="R83">
         <f t="shared" si="10"/>
-        <v>0.999999999999999</v>
+        <v>9.9999999999999893</v>
       </c>
       <c r="T83">
         <f t="shared" si="11"/>
-        <v>0.64384829258687659</v>
+        <v>3.6438482925868736</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
@@ -10364,11 +10512,11 @@
       </c>
       <c r="R84">
         <f t="shared" si="10"/>
-        <v>0.99999999999999933</v>
+        <v>9.9999999999999929</v>
       </c>
       <c r="T84">
         <f t="shared" si="11"/>
-        <v>0.6271880305300902</v>
+        <v>3.6271880305300876</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
@@ -10423,11 +10571,11 @@
       </c>
       <c r="R85">
         <f t="shared" si="10"/>
-        <v>0.99999999999999967</v>
+        <v>9.9999999999999964</v>
       </c>
       <c r="T85">
         <f t="shared" si="11"/>
-        <v>0.611349153935832</v>
+        <v>3.6113491539358313</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
@@ -10482,11 +10630,11 @@
       </c>
       <c r="R86">
         <f t="shared" si="10"/>
-        <v>0.99999999999999978</v>
+        <v>9.9999999999999982</v>
       </c>
       <c r="T86">
         <f t="shared" si="11"/>
-        <v>0.59629880982454431</v>
+        <v>3.5962988098245443</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
@@ -10541,11 +10689,11 @@
       </c>
       <c r="R87">
         <f t="shared" si="10"/>
-        <v>0.99999999999999989</v>
+        <v>9.9999999999999982</v>
       </c>
       <c r="T87">
         <f t="shared" si="11"/>
-        <v>0.582004642101006</v>
+        <v>3.5820046421010052</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
@@ -10600,11 +10748,11 @@
       </c>
       <c r="R88">
         <f t="shared" si="10"/>
-        <v>0.99999999999999989</v>
+        <v>10</v>
       </c>
       <c r="T88">
         <f>SUM(R88*O88,L88*I88,F88*C88)/SUM(O88,I88,C88)</f>
-        <v>0.56843488228687644</v>
+        <v>3.5684348822868763</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
@@ -10659,11 +10807,11 @@
       </c>
       <c r="R89">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T89">
         <f t="shared" ref="T89:T108" si="12">SUM(R89*O89,L89*I89,F89*C89)/SUM(O89,I89,C89)</f>
-        <v>0.55555842710197223</v>
+        <v>3.5555584271019725</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
@@ -10718,11 +10866,11 @@
       </c>
       <c r="R90">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T90">
         <f t="shared" si="12"/>
-        <v>0.54334490380349765</v>
+        <v>3.5433449038034972</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
@@ -10777,11 +10925,11 @@
       </c>
       <c r="R91">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T91">
         <f t="shared" si="12"/>
-        <v>0.53176472421278376</v>
+        <v>3.5317647242127834</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
@@ -10836,11 +10984,11 @@
       </c>
       <c r="R92">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T92">
         <f t="shared" si="12"/>
-        <v>0.52078912836086866</v>
+        <v>3.5207891283608688</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
@@ -10895,11 +11043,11 @@
       </c>
       <c r="R93">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T93">
         <f t="shared" si="12"/>
-        <v>0.51039021867116441</v>
+        <v>3.510390218671164</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
@@ -10954,11 +11102,11 @@
       </c>
       <c r="R94">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T94">
         <f t="shared" si="12"/>
-        <v>0.50054098557263416</v>
+        <v>3.5005409855726342</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
@@ -11013,11 +11161,11 @@
       </c>
       <c r="R95">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T95">
         <f t="shared" si="12"/>
-        <v>0.49121532540309193</v>
+        <v>3.4912153254030915</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
@@ -11072,11 +11220,11 @@
       </c>
       <c r="R96">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T96">
         <f t="shared" si="12"/>
-        <v>0.48238805142175645</v>
+        <v>3.4823880514217564</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
@@ -11131,11 +11279,11 @@
       </c>
       <c r="R97">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T97">
         <f t="shared" si="12"/>
-        <v>0.47403489870501653</v>
+        <v>3.4740348987050171</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
@@ -11190,11 +11338,11 @@
       </c>
       <c r="R98">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T98">
         <f t="shared" si="12"/>
-        <v>0.46613252365114483</v>
+        <v>3.4661325236511442</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
@@ -11249,11 +11397,11 @@
       </c>
       <c r="R99">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T99">
         <f t="shared" si="12"/>
-        <v>0.45865849876980375</v>
+        <v>3.4586584987698035</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
@@ -11308,11 +11456,11 @@
       </c>
       <c r="R100">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T100">
         <f t="shared" si="12"/>
-        <v>0.4515913033817423</v>
+        <v>3.4515913033817429</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
@@ -11367,11 +11515,11 @@
       </c>
       <c r="R101">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T101">
         <f t="shared" si="12"/>
-        <v>0.44491031080397536</v>
+        <v>3.4449103108039751</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.2">
@@ -11426,11 +11574,11 @@
       </c>
       <c r="R102">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T102">
         <f t="shared" si="12"/>
-        <v>0.43859577254669757</v>
+        <v>3.4385957725466976</v>
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
@@ -11485,11 +11633,11 @@
       </c>
       <c r="R103">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T103">
         <f t="shared" si="12"/>
-        <v>0.4326288000007425</v>
+        <v>3.4326288000007423</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.2">
@@ -11544,11 +11692,11 @@
       </c>
       <c r="R104">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T104">
         <f t="shared" si="12"/>
-        <v>0.42699134404897937</v>
+        <v>3.4269913440489792</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
@@ -11603,11 +11751,11 @@
       </c>
       <c r="R105">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T105">
         <f t="shared" si="12"/>
-        <v>0.42166617299192932</v>
+        <v>3.4216661729919298</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
@@ -11662,11 +11810,11 @@
       </c>
       <c r="R106">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T106">
         <f t="shared" si="12"/>
-        <v>0.41663684913727966</v>
+        <v>3.4166368491372796</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.2">
@@ -11721,11 +11869,11 @@
       </c>
       <c r="R107">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T107">
         <f t="shared" si="12"/>
-        <v>0.41188770436499372</v>
+        <v>3.4118877043649936</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.2">
@@ -11780,11 +11928,11 @@
       </c>
       <c r="R108">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T108">
         <f t="shared" si="12"/>
-        <v>0.40740381494440148</v>
+        <v>3.4074038149444008</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.2">
@@ -11823,7 +11971,7 @@
       </c>
       <c r="R109">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.2">
@@ -11862,7 +12010,7 @@
       </c>
       <c r="R110">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.2">
@@ -11901,7 +12049,7 @@
       </c>
       <c r="R111">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.2">
@@ -11940,7 +12088,7 @@
       </c>
       <c r="R112">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
@@ -11979,7 +12127,7 @@
       </c>
       <c r="R113">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
@@ -12018,7 +12166,7 @@
       </c>
       <c r="R114">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
@@ -12057,7 +12205,7 @@
       </c>
       <c r="R115">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
@@ -12096,7 +12244,7 @@
       </c>
       <c r="R116">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
@@ -12135,7 +12283,7 @@
       </c>
       <c r="R117">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
@@ -12174,7 +12322,7 @@
       </c>
       <c r="R118">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
@@ -12213,7 +12361,7 @@
       </c>
       <c r="R119">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
@@ -12252,7 +12400,7 @@
       </c>
       <c r="R120">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
@@ -12291,7 +12439,7 @@
       </c>
       <c r="R121">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.2">
@@ -12330,7 +12478,7 @@
       </c>
       <c r="R122">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.2">
@@ -12369,7 +12517,7 @@
       </c>
       <c r="R123">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.2">
@@ -12408,7 +12556,7 @@
       </c>
       <c r="R124">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.2">
@@ -12447,7 +12595,7 @@
       </c>
       <c r="R125">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.2">
@@ -12486,7 +12634,7 @@
       </c>
       <c r="R126">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.2">
@@ -12525,7 +12673,7 @@
       </c>
       <c r="R127">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.2">
@@ -12564,7 +12712,7 @@
       </c>
       <c r="R128">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.2">
@@ -12603,7 +12751,7 @@
       </c>
       <c r="R129">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
@@ -12642,7 +12790,7 @@
       </c>
       <c r="R130">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.2">
@@ -12660,7 +12808,7 @@
       </c>
       <c r="R131">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.2">
@@ -12678,7 +12826,7 @@
       </c>
       <c r="R132">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.2">
@@ -12696,7 +12844,7 @@
       </c>
       <c r="R133">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.2">
@@ -12714,7 +12862,7 @@
       </c>
       <c r="R134">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.2">
@@ -12732,7 +12880,7 @@
       </c>
       <c r="R135">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.2">
@@ -12750,7 +12898,7 @@
       </c>
       <c r="R136">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.2">
@@ -12768,7 +12916,7 @@
       </c>
       <c r="R137">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.2">
@@ -12785,8 +12933,8 @@
         <v>0.5</v>
       </c>
       <c r="R138">
-        <f t="shared" ref="R138:R201" si="13">1-1/(1+EXP(-Q138*(P138-N138)))</f>
-        <v>1</v>
+        <f t="shared" ref="R138:R201" si="13">10-10/(1+EXP(-Q138*(P138-N138)))</f>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.2">
@@ -12804,7 +12952,7 @@
       </c>
       <c r="R139">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.2">
@@ -12822,7 +12970,7 @@
       </c>
       <c r="R140">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.2">
@@ -12840,7 +12988,7 @@
       </c>
       <c r="R141">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.2">
@@ -12858,7 +13006,7 @@
       </c>
       <c r="R142">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.2">
@@ -12876,7 +13024,7 @@
       </c>
       <c r="R143">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.2">
@@ -12894,7 +13042,7 @@
       </c>
       <c r="R144">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="14:18" x14ac:dyDescent="0.2">
@@ -12912,7 +13060,7 @@
       </c>
       <c r="R145">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="14:18" x14ac:dyDescent="0.2">
@@ -12930,7 +13078,7 @@
       </c>
       <c r="R146">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="14:18" x14ac:dyDescent="0.2">
@@ -12948,7 +13096,7 @@
       </c>
       <c r="R147">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="14:18" x14ac:dyDescent="0.2">
@@ -12966,7 +13114,7 @@
       </c>
       <c r="R148">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="14:18" x14ac:dyDescent="0.2">
@@ -12984,7 +13132,7 @@
       </c>
       <c r="R149">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="14:18" x14ac:dyDescent="0.2">
@@ -13002,7 +13150,7 @@
       </c>
       <c r="R150">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="14:18" x14ac:dyDescent="0.2">
@@ -13020,7 +13168,7 @@
       </c>
       <c r="R151">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="14:18" x14ac:dyDescent="0.2">
@@ -13038,7 +13186,7 @@
       </c>
       <c r="R152">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="14:18" x14ac:dyDescent="0.2">
@@ -13056,7 +13204,7 @@
       </c>
       <c r="R153">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="14:18" x14ac:dyDescent="0.2">
@@ -13074,7 +13222,7 @@
       </c>
       <c r="R154">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="14:18" x14ac:dyDescent="0.2">
@@ -13092,7 +13240,7 @@
       </c>
       <c r="R155">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="14:18" x14ac:dyDescent="0.2">
@@ -13110,7 +13258,7 @@
       </c>
       <c r="R156">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="14:18" x14ac:dyDescent="0.2">
@@ -13128,7 +13276,7 @@
       </c>
       <c r="R157">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="14:18" x14ac:dyDescent="0.2">
@@ -13146,7 +13294,7 @@
       </c>
       <c r="R158">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="14:18" x14ac:dyDescent="0.2">
@@ -13164,7 +13312,7 @@
       </c>
       <c r="R159">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="14:18" x14ac:dyDescent="0.2">
@@ -13182,7 +13330,7 @@
       </c>
       <c r="R160">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="14:18" x14ac:dyDescent="0.2">
@@ -13200,7 +13348,7 @@
       </c>
       <c r="R161">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="14:18" x14ac:dyDescent="0.2">
@@ -13218,7 +13366,7 @@
       </c>
       <c r="R162">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="14:18" x14ac:dyDescent="0.2">
@@ -13236,7 +13384,7 @@
       </c>
       <c r="R163">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="14:18" x14ac:dyDescent="0.2">
@@ -13254,7 +13402,7 @@
       </c>
       <c r="R164">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="14:18" x14ac:dyDescent="0.2">
@@ -13272,7 +13420,7 @@
       </c>
       <c r="R165">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="14:18" x14ac:dyDescent="0.2">
@@ -13290,7 +13438,7 @@
       </c>
       <c r="R166">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="14:18" x14ac:dyDescent="0.2">
@@ -13308,7 +13456,7 @@
       </c>
       <c r="R167">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="14:18" x14ac:dyDescent="0.2">
@@ -13326,7 +13474,7 @@
       </c>
       <c r="R168">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="14:18" x14ac:dyDescent="0.2">
@@ -13344,7 +13492,7 @@
       </c>
       <c r="R169">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="14:18" x14ac:dyDescent="0.2">
@@ -13362,7 +13510,7 @@
       </c>
       <c r="R170">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="14:18" x14ac:dyDescent="0.2">
@@ -13380,7 +13528,7 @@
       </c>
       <c r="R171">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="14:18" x14ac:dyDescent="0.2">
@@ -13398,7 +13546,7 @@
       </c>
       <c r="R172">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="14:18" x14ac:dyDescent="0.2">
@@ -13416,7 +13564,7 @@
       </c>
       <c r="R173">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="14:18" x14ac:dyDescent="0.2">
@@ -13434,7 +13582,7 @@
       </c>
       <c r="R174">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="14:18" x14ac:dyDescent="0.2">
@@ -13452,7 +13600,7 @@
       </c>
       <c r="R175">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="14:18" x14ac:dyDescent="0.2">
@@ -13470,7 +13618,7 @@
       </c>
       <c r="R176">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="14:18" x14ac:dyDescent="0.2">
@@ -13488,7 +13636,7 @@
       </c>
       <c r="R177">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="14:18" x14ac:dyDescent="0.2">
@@ -13506,7 +13654,7 @@
       </c>
       <c r="R178">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" spans="14:18" x14ac:dyDescent="0.2">
@@ -13524,7 +13672,7 @@
       </c>
       <c r="R179">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="14:18" x14ac:dyDescent="0.2">
@@ -13542,7 +13690,7 @@
       </c>
       <c r="R180">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="14:18" x14ac:dyDescent="0.2">
@@ -13560,7 +13708,7 @@
       </c>
       <c r="R181">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="14:18" x14ac:dyDescent="0.2">
@@ -13578,7 +13726,7 @@
       </c>
       <c r="R182">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="14:18" x14ac:dyDescent="0.2">
@@ -13596,7 +13744,7 @@
       </c>
       <c r="R183">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="14:18" x14ac:dyDescent="0.2">
@@ -13614,7 +13762,7 @@
       </c>
       <c r="R184">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="14:18" x14ac:dyDescent="0.2">
@@ -13632,7 +13780,7 @@
       </c>
       <c r="R185">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="14:18" x14ac:dyDescent="0.2">
@@ -13650,7 +13798,7 @@
       </c>
       <c r="R186">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="14:18" x14ac:dyDescent="0.2">
@@ -13668,7 +13816,7 @@
       </c>
       <c r="R187">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="14:18" x14ac:dyDescent="0.2">
@@ -13686,7 +13834,7 @@
       </c>
       <c r="R188">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="14:18" x14ac:dyDescent="0.2">
@@ -13704,7 +13852,7 @@
       </c>
       <c r="R189">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="14:18" x14ac:dyDescent="0.2">
@@ -13722,7 +13870,7 @@
       </c>
       <c r="R190">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" spans="14:18" x14ac:dyDescent="0.2">
@@ -13740,7 +13888,7 @@
       </c>
       <c r="R191">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="14:18" x14ac:dyDescent="0.2">
@@ -13758,7 +13906,7 @@
       </c>
       <c r="R192">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="14:18" x14ac:dyDescent="0.2">
@@ -13776,7 +13924,7 @@
       </c>
       <c r="R193">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="14:18" x14ac:dyDescent="0.2">
@@ -13794,7 +13942,7 @@
       </c>
       <c r="R194">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" spans="14:18" x14ac:dyDescent="0.2">
@@ -13812,7 +13960,7 @@
       </c>
       <c r="R195">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="14:18" x14ac:dyDescent="0.2">
@@ -13830,7 +13978,7 @@
       </c>
       <c r="R196">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="14:18" x14ac:dyDescent="0.2">
@@ -13848,7 +13996,7 @@
       </c>
       <c r="R197">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="14:18" x14ac:dyDescent="0.2">
@@ -13866,7 +14014,7 @@
       </c>
       <c r="R198">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="14:18" x14ac:dyDescent="0.2">
@@ -13884,7 +14032,7 @@
       </c>
       <c r="R199">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="14:18" x14ac:dyDescent="0.2">
@@ -13902,7 +14050,7 @@
       </c>
       <c r="R200">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="14:18" x14ac:dyDescent="0.2">
@@ -13920,7 +14068,7 @@
       </c>
       <c r="R201">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" spans="14:18" x14ac:dyDescent="0.2">
@@ -13937,8 +14085,8 @@
         <v>0.5</v>
       </c>
       <c r="R202">
-        <f t="shared" ref="R202:R209" si="14">1-1/(1+EXP(-Q202*(P202-N202)))</f>
-        <v>1</v>
+        <f t="shared" ref="R202:R209" si="14">10-10/(1+EXP(-Q202*(P202-N202)))</f>
+        <v>10</v>
       </c>
     </row>
     <row r="203" spans="14:18" x14ac:dyDescent="0.2">
@@ -13956,7 +14104,7 @@
       </c>
       <c r="R203">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" spans="14:18" x14ac:dyDescent="0.2">
@@ -13974,7 +14122,7 @@
       </c>
       <c r="R204">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205" spans="14:18" x14ac:dyDescent="0.2">
@@ -13992,7 +14140,7 @@
       </c>
       <c r="R205">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="206" spans="14:18" x14ac:dyDescent="0.2">
@@ -14010,7 +14158,7 @@
       </c>
       <c r="R206">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="207" spans="14:18" x14ac:dyDescent="0.2">
@@ -14028,7 +14176,7 @@
       </c>
       <c r="R207">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="208" spans="14:18" x14ac:dyDescent="0.2">
@@ -14046,7 +14194,7 @@
       </c>
       <c r="R208">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="209" spans="14:18" x14ac:dyDescent="0.2">
@@ -14064,7 +14212,7 @@
       </c>
       <c r="R209">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>